<commit_message>
Line Clipping Updated, More to do
Signed-off-by: Ian O Regan <Ian.ORegan@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/MatrixTests.xlsx
+++ b/MatrixTests.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Translation</t>
   </si>
@@ -72,6 +73,111 @@
   </si>
   <si>
     <t>Rotation</t>
+  </si>
+  <si>
+    <t>perspective projection</t>
+  </si>
+  <si>
+    <t>divide by -z</t>
+  </si>
+  <si>
+    <t>Efficiency of Matrices</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>vetrices</t>
+  </si>
+  <si>
+    <t>Transform</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Projection</t>
+  </si>
+  <si>
+    <t>Viewing</t>
+  </si>
+  <si>
+    <t>Matrices</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>4 mult 3 add</t>
+  </si>
+  <si>
+    <t>16 mult 12 add</t>
+  </si>
+  <si>
+    <t>Transfomations</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>160,000 mult</t>
+  </si>
+  <si>
+    <t>120,000 add</t>
+  </si>
+  <si>
+    <t>5 transforms</t>
+  </si>
+  <si>
+    <t>800,000 mult</t>
+  </si>
+  <si>
+    <t>600,000 add</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>64 mult</t>
+  </si>
+  <si>
+    <t>42 add</t>
+  </si>
+  <si>
+    <t>5 matrices</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>256 mult</t>
+  </si>
+  <si>
+    <t>192 add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super </t>
+  </si>
+  <si>
+    <t>16 mult</t>
+  </si>
+  <si>
+    <t>12 add</t>
+  </si>
+  <si>
+    <t>Total calulations</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -95,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -227,11 +333,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,6 +399,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,6 +426,926 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$1:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.75651890021989798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.15646826398338626</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.24293233128235328</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.85527936325825316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.72153269495108174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.10288737347197416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.19177841929556333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.82355613750085566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$1:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11565606396437388</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.13054737167682309</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.37481502955364127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.14128008318834462</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18311470418853781</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.5705166335482618E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.32789696948451641</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.2588793035801036E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-57CF-4B51-8C6F-90A88AED4978}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1148754495"/>
+        <c:axId val="1148751583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1148754495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1148751583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1148751583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1148754495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,15 +1611,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y20"/>
+  <dimension ref="B2:AI53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16:R19"/>
+    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="24" width="9.140625" style="4"/>
+    <col min="25" max="25" width="11.28515625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="11" style="4" customWidth="1"/>
+    <col min="27" max="28" width="9.140625" style="4"/>
+    <col min="29" max="29" width="11.7109375" style="4" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
@@ -818,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
@@ -869,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="e">
         <f>-Sin a</f>
         <v>#NAME?</v>
@@ -921,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>0</v>
       </c>
@@ -968,9 +2029,1029 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="3:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="S24" s="11"/>
+      <c r="T24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="8"/>
+    </row>
+    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="I25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S25" s="12"/>
+      <c r="T25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U25" s="16">
+        <v>10000</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG25" s="14"/>
+      <c r="AH25" s="14"/>
+      <c r="AI25" s="9"/>
+    </row>
+    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="S26" s="12"/>
+      <c r="T26" s="14">
+        <v>3</v>
+      </c>
+      <c r="U26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG26" s="14"/>
+      <c r="AH26" s="14"/>
+      <c r="AI26" s="9"/>
+    </row>
+    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="I27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="S27" s="12"/>
+      <c r="T27" s="14">
+        <v>1</v>
+      </c>
+      <c r="U27" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="V27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG27" s="14"/>
+      <c r="AH27" s="14"/>
+      <c r="AI27" s="9"/>
+    </row>
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+      <c r="S28" s="12"/>
+      <c r="T28" s="14">
+        <v>1</v>
+      </c>
+      <c r="U28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG28" s="14"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="9"/>
+    </row>
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+      <c r="S29" s="12"/>
+      <c r="T29" s="14">
+        <v>5</v>
+      </c>
+      <c r="U29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V29" s="14"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="14"/>
+      <c r="AC29" s="14"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="14"/>
+      <c r="AF29" s="14"/>
+      <c r="AG29" s="14"/>
+      <c r="AH29" s="14"/>
+      <c r="AI29" s="9"/>
+    </row>
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
+        <v>-1</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="S30" s="12"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+      <c r="AB30" s="14"/>
+      <c r="AC30" s="14"/>
+      <c r="AD30" s="14"/>
+      <c r="AE30" s="14"/>
+      <c r="AF30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="14"/>
+      <c r="AI30" s="9"/>
+    </row>
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="S31" s="12"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14"/>
+      <c r="AB31" s="14"/>
+      <c r="AC31" s="14"/>
+      <c r="AD31" s="14"/>
+      <c r="AE31" s="14"/>
+      <c r="AF31" s="14"/>
+      <c r="AG31" s="14"/>
+      <c r="AH31" s="14"/>
+      <c r="AI31" s="9"/>
+    </row>
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="S32" s="12"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="14"/>
+      <c r="AB32" s="14"/>
+      <c r="AC32" s="14"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="14"/>
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="14"/>
+      <c r="AH32" s="14"/>
+      <c r="AI32" s="9"/>
+    </row>
+    <row r="33" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S33" s="12"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="16">
+        <v>10000</v>
+      </c>
+      <c r="Z33" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA33" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB33" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC33" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="14"/>
+      <c r="AG33" s="14"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="9"/>
+    </row>
+    <row r="34" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S34" s="12"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="9"/>
+    </row>
+    <row r="35" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S35" s="12"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+      <c r="AB35" s="14"/>
+      <c r="AC35" s="14"/>
+      <c r="AD35" s="14"/>
+      <c r="AE35" s="14"/>
+      <c r="AF35" s="14"/>
+      <c r="AG35" s="14"/>
+      <c r="AH35" s="14"/>
+      <c r="AI35" s="9"/>
+    </row>
+    <row r="36" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S36" s="12"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB36" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC36" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="9"/>
+    </row>
+    <row r="37" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S37" s="12"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="9"/>
+    </row>
+    <row r="38" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S38" s="12"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="14"/>
+      <c r="AF38" s="14"/>
+      <c r="AG38" s="14"/>
+      <c r="AH38" s="14"/>
+      <c r="AI38" s="9"/>
+    </row>
+    <row r="39" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S39" s="12"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="14"/>
+      <c r="X39" s="14"/>
+      <c r="Y39" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI39" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S40" s="12"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S41" s="12"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="14"/>
+      <c r="AD41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="14"/>
+      <c r="AI41" s="9"/>
+    </row>
+    <row r="42" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S42" s="12"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC42" s="14"/>
+      <c r="AD42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH42" s="14"/>
+      <c r="AI42" s="9"/>
+    </row>
+    <row r="43" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S43" s="12"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="9"/>
+    </row>
+    <row r="44" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S44" s="12"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z44" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA44" s="14"/>
+      <c r="AB44" s="14"/>
+      <c r="AC44" s="14"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="14"/>
+      <c r="AF44" s="14"/>
+      <c r="AG44" s="14"/>
+      <c r="AH44" s="14"/>
+      <c r="AI44" s="9"/>
+    </row>
+    <row r="45" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S45" s="12"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14">
+        <v>4</v>
+      </c>
+      <c r="AA45" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB45" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC45" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD45" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE45" s="14"/>
+      <c r="AF45" s="14"/>
+      <c r="AG45" s="14"/>
+      <c r="AH45" s="14"/>
+      <c r="AI45" s="9"/>
+    </row>
+    <row r="46" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S46" s="12"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+      <c r="Z46" s="14"/>
+      <c r="AA46" s="14"/>
+      <c r="AB46" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC46" s="14"/>
+      <c r="AD46" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE46" s="14"/>
+      <c r="AF46" s="14"/>
+      <c r="AG46" s="14"/>
+      <c r="AH46" s="14"/>
+      <c r="AI46" s="9"/>
+    </row>
+    <row r="47" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S47" s="12"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="14"/>
+      <c r="AA47" s="14"/>
+      <c r="AB47" s="14"/>
+      <c r="AC47" s="14"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="14"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="14"/>
+      <c r="AH47" s="14"/>
+      <c r="AI47" s="9"/>
+    </row>
+    <row r="48" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S48" s="12"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="14"/>
+      <c r="AA48" s="14"/>
+      <c r="AB48" s="14"/>
+      <c r="AC48" s="14"/>
+      <c r="AD48" s="14"/>
+      <c r="AE48" s="14"/>
+      <c r="AF48" s="14"/>
+      <c r="AG48" s="14"/>
+      <c r="AH48" s="14"/>
+      <c r="AI48" s="9"/>
+    </row>
+    <row r="49" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S49" s="12"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y49" s="16">
+        <v>10000</v>
+      </c>
+      <c r="Z49" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA49" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB49" s="14"/>
+      <c r="AC49" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD49" s="16">
+        <v>160000</v>
+      </c>
+      <c r="AE49" s="14"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
+      <c r="AH49" s="14"/>
+      <c r="AI49" s="9"/>
+    </row>
+    <row r="50" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S50" s="12"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="14"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="14"/>
+      <c r="X50" s="14"/>
+      <c r="Y50" s="14"/>
+      <c r="Z50" s="14"/>
+      <c r="AA50" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB50" s="14"/>
+      <c r="AC50" s="14"/>
+      <c r="AD50" s="16">
+        <v>120000</v>
+      </c>
+      <c r="AE50" s="14"/>
+      <c r="AF50" s="14"/>
+      <c r="AG50" s="14"/>
+      <c r="AH50" s="14"/>
+      <c r="AI50" s="9"/>
+    </row>
+    <row r="51" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S51" s="12"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="14"/>
+      <c r="AA51" s="14"/>
+      <c r="AB51" s="14"/>
+      <c r="AC51" s="14"/>
+      <c r="AD51" s="14"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="14"/>
+      <c r="AI51" s="9"/>
+    </row>
+    <row r="52" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S52" s="12"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="14"/>
+      <c r="X52" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y52" s="14"/>
+      <c r="Z52" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA52" s="14"/>
+      <c r="AB52" s="16">
+        <v>160000</v>
+      </c>
+      <c r="AC52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD52" s="14">
+        <v>256</v>
+      </c>
+      <c r="AE52" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF52" s="16">
+        <v>160256</v>
+      </c>
+      <c r="AG52" s="14"/>
+      <c r="AH52" s="14"/>
+      <c r="AI52" s="9"/>
+    </row>
+    <row r="53" spans="19:35" x14ac:dyDescent="0.25">
+      <c r="S53" s="13"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="17"/>
+      <c r="Y53" s="17"/>
+      <c r="Z53" s="17"/>
+      <c r="AA53" s="17"/>
+      <c r="AB53" s="18">
+        <v>120000</v>
+      </c>
+      <c r="AC53" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD53" s="17">
+        <v>192</v>
+      </c>
+      <c r="AE53" s="17"/>
+      <c r="AF53" s="18">
+        <v>120192</v>
+      </c>
+      <c r="AG53" s="17"/>
+      <c r="AH53" s="17"/>
+      <c r="AI53" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>-38.025840000000002</v>
+      </c>
+      <c r="B1" s="4">
+        <v>5.8133629999999998</v>
+      </c>
+      <c r="C1" s="4">
+        <v>50.264229999999998</v>
+      </c>
+      <c r="E1">
+        <f>A1/C1</f>
+        <v>-0.75651890021989798</v>
+      </c>
+      <c r="F1">
+        <f>B1/C1</f>
+        <v>0.11565606396437388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>-8.3571639999999991</v>
+      </c>
+      <c r="B2" s="4">
+        <v>-6.9726970000000001</v>
+      </c>
+      <c r="C2" s="4">
+        <v>53.411239999999999</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E8" si="0">A2/C2</f>
+        <v>-0.15646826398338626</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F8" si="1">B2/C2</f>
+        <v>-0.13054737167682309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>-12.83807</v>
+      </c>
+      <c r="B3" s="4">
+        <v>-19.807580000000002</v>
+      </c>
+      <c r="C3" s="4">
+        <v>52.84628</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-0.24293233128235328</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>-0.37481502955364127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>-42.50676</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-7.0215170000000002</v>
+      </c>
+      <c r="C4" s="4">
+        <v>49.699269999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>-0.85527936325825316</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>-0.14128008318834462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>-34.980539999999998</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8.8775619999999993</v>
+      </c>
+      <c r="C5" s="4">
+        <v>48.480879999999999</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-0.72153269495108174</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.18311470418853781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>-5.311858</v>
+      </c>
+      <c r="B6" s="4">
+        <v>-3.9084979999999998</v>
+      </c>
+      <c r="C6" s="4">
+        <v>51.627890000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-0.10288737347197416</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>-7.5705166335482618E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>-9.7927680000000006</v>
+      </c>
+      <c r="B7" s="4">
+        <v>-16.743379999999998</v>
+      </c>
+      <c r="C7" s="4">
+        <v>51.062930000000001</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-0.19177841929556333</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>-0.32789696948451641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>-39.461449999999999</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-3.9573179999999999</v>
+      </c>
+      <c r="C8" s="4">
+        <v>47.91592</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-0.82355613750085566</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>-8.2588793035801036E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>